<commit_message>
Add benchmark answers and update test dataset
</commit_message>
<xml_diff>
--- a/benchmark/test-dataset.xlsx
+++ b/benchmark/test-dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidgil/Sites/enterprise-rag/benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E84C721-AF99-334B-95E7-A708BF326F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B702B767-5DAD-F04F-A545-8857F1E75871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12920" yWindow="-26520" windowWidth="48400" windowHeight="26520" xr2:uid="{6A3309C2-77CF-B84D-961D-4A9B63FD3B6A}"/>
+    <workbookView xWindow="-5380" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{6A3309C2-77CF-B84D-961D-4A9B63FD3B6A}"/>
   </bookViews>
   <sheets>
     <sheet name="test-dataset" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Question</t>
   </si>
@@ -200,6 +200,121 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>LLM Answer</t>
+  </si>
+  <si>
+    <t>Based on the retrieved documents, Apple's total net sales for fiscal year 2024 were $391,035 million. This figure represents their total revenue for that period. 
+Additionally, Document 2 notes that there was $7.7 billion of revenue recognized in 2024 that had been included in deferred revenue as of September 30, 2023. However, the "Total net sales" amount already incorporates this recognized revenue, so it does not require further adjustment for total revenue calculation.
+Therefore, Apple's total revenue for fiscal year 2024 was $391,035 million.</t>
+  </si>
+  <si>
+    <t>Apple's total net sales increased by 2% from 2023 to 2024. In 2023, the total net sales were $383,285 million, and in 2024, they rose to $391,035 million. This increase reflects a positive change in revenue for Apple over that period.</t>
+  </si>
+  <si>
+    <t>Based on the provided documents, Apple Inc.'s total net sales for 2023 were $383,285 million, and for 2024 they were $391,035 million. To calculate the revenue growth rate from 2023 to 2024:
+\[
+\text{Growth Rate} = \left(\frac{\text{Net Sales in 2024} - \text{Net Sales in 2023}}{\text{Net Sales in 2023}}\right) \times 100
+\]
+\[
+= \left(\frac{391,035 - 383,285}{383,285}\right) \times 100
+\]
+\[
+= \left(\frac{7,750}{383,285}\right) \times 100 \approx 2.02\%
+\]
+Therefore, Apple's revenue growth rate between 2023 and 2024 was approximately 2%.</t>
+  </si>
+  <si>
+    <t>To calculate Apple's revenue growth rate between 2022 and 2023, we use the formula for percentage change:
+\[
+\text{Growth Rate} = \left( \frac{\text{Revenue in 2023} - \text{Revenue in 2022}}{\text{Revenue in 2022}} \right) \times 100
+\]
+From Document 1, we have:
+- Total net sales for 2023: $383,285 million
+- Total net sales for 2022: $394,328 million
+Plug these values into the formula:
+\[
+\text{Growth Rate} = \left( \frac{383,285 - 394,328}{394,328} \right) \times 100
+\]
+\[
+\text{Growth Rate} = \left( \frac{-11,043}{394,328} \right) \times 100
+\]
+\[
+\text{Growth Rate} \approx -2.8\%
+\]
+Therefore, Apple's revenue growth rate between 2022 and 2023 was approximately \(-2.8\%\).</t>
+  </si>
+  <si>
+    <t>Based on the provided documents, Apple's total net sales for the fiscal year 2022 were $394,328 million. This information is found in both Document 1 and Document 2 under the "Total Net Sales" section for the years 2024, 2023, and 2022.</t>
+  </si>
+  <si>
+    <t>Based on the retrieved documents provided, I do not see any specific information regarding the number of employees at Apple Inc. Therefore, I am unable to provide an answer to your question with the given documents. If you are looking for current and accurate figures on Apple's workforce size, I recommend checking Apple's official website or recent reports from credible sources like financial news outlets.</t>
+  </si>
+  <si>
+    <t>Microsoft's total revenue for fiscal year 2024 was $245.122 billion, as detailed in Document 1 under "Revenue, classified by significant product and service offerings."</t>
+  </si>
+  <si>
+    <t>The total revenue for Microsoft in fiscal year 2024 increased by $33.2 billion, which corresponds to a growth of 16% compared to fiscal year 2023. This information is provided in Document 1 under the section "Fiscal Year 2024 Compared with Fiscal Year 2023."</t>
+  </si>
+  <si>
+    <t>The Productivity and Business Processes segment generated $60,184 million in unearned revenue as of June 30, 2024. However, to find the total revenue for this segment in 2024, we should refer to Document 3.
+According to Document 3:
+- Office products and cloud services revenue was $54,875 million.
+- LinkedIn revenue was $16,372 million.
+- Dynamics products and cloud services revenue was $6,481 million.
+To calculate the total revenue for the Productivity and Business Processes segment in 2024, sum these amounts:
+\[ 
+54,875 + 16,372 + 6,481 = 77,728 \text{ million}
+\]
+Therefore, the Productivity and Business Processes segment generated $77,728 million in revenue in 2024.</t>
+  </si>
+  <si>
+    <t>The Intelligent Cloud segment generated $97,726 million in revenue for the fiscal year ended June 30, 2024. This information is found in Document 2 under the section "Revenue, classified by significant product and service offerings." The breakdown includes Server products and cloud services, which are part of this segment's revenue.</t>
+  </si>
+  <si>
+    <t>Microsoft's total gross margin for fiscal year 2024 was $171,008 million. This information is provided in Document 2 under the SUMMARY RESULTS OF OPERATIONS section.
+To provide additional context, according to Document 3, the breakdown of gross margin into products and services for 2024 are as follows:
+- Products Gross Margin: $109,633 million
+- Services Gross Margin: $71,050 million
+These figures combined total the overall gross margin reported in fiscal year 2024.</t>
+  </si>
+  <si>
+    <t>Microsoft's operating income for the fiscal year 2024 was $109.4 billion. This information is found in Document 3 under the "Operating Income" section for the year ended June 30, 2024.</t>
+  </si>
+  <si>
+    <t>Microsoft's net income for the fiscal year ended June 30, 2024, was $88.136 billion. This information is found in Document 2 under the "Income Statements" section for the year 2024.</t>
+  </si>
+  <si>
+    <t>Based on the retrieved documents, there are two sets of financial data for Microsoft in the fiscal year 2024. 
+From Document 1, which appears to be a part of Note 3 - Earnings Per Share:
+- Basic earnings per share (EPS) for 2024 is $6.11
+- Diluted earnings per share (EPS) for 2024 is $6.08
+From Document 2, which summarizes the results of operations:
+- Diluted EPS for 2024 is $11.80 
+The discrepancy suggests that these documents might pertain to different segments or aspects of Microsoft's financial reporting. To provide a comprehensive answer based on this data, Microsoft’s diluted earnings per share (EPS) for fiscal year 2024 could be reported as both $6.08 and $11.80 depending on the context:
+- $6.08 from Document 1
+- $11.80 from Document 2
+Without additional context to reconcile these differences, it is unclear which figure should be used universally across all of Microsoft's operations for fiscal year 2024.</t>
+  </si>
+  <si>
+    <t>Based on the retrieved documents provided, there is information regarding Apple's total net sales for fiscal year 2024, which amounted to $391.035 billion. However, there is no information available about Microsoft's total revenue for fiscal year 2024 within these documents.
+Without additional data or documents that include Microsoft's financial figures for the same period, I am unable to determine which company had higher total revenue in fiscal year 2024. If you have access to Microsoft's financial reports or other relevant sources, you could compare their total revenue for fiscal year 2024 against Apple's $391.035 billion to answer this question accurately.</t>
+  </si>
+  <si>
+    <t>Based on the documents provided, I only have information about Apple's financial performance for fiscal year 2024. The documents do not provide any data regarding Microsoft's revenue growth rate for the same period. Therefore, I cannot determine which company had a higher revenue growth rate in fiscal year 2024 based solely on these documents.</t>
+  </si>
+  <si>
+    <t>Based on the provided documents, we can determine which segment contributed the most revenue for Microsoft but not for Apple. The relevant document provides detailed financial information about Microsoft's segments:
+- **Productivity and Business Processes**: $77,728 million
+- **Intelligent Cloud**: $105,362 million
+- **More Personal Computing**: $62,032 million
+For the year ended June 30, 2024, the "Intelligent Cloud" segment contributed the most revenue for Microsoft, amounting to $105,362 million.
+Regarding Apple Inc., no specific financial data about its segments was provided in the retrieved documents. Therefore, I do not have enough information to determine which segment contributed the most revenue for Apple based on these documents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Based on the provided documents, there is no specific information about the operating income for either Apple or Microsoft in fiscal year 2024. The documents detail revenue figures and segment performance but do not include direct data on operating income. To determine which company had higher operating income, you would need access to their respective financial statements from that fiscal year, particularly focusing on their consolidated income statements where operating income is typically reported.</t>
   </si>
 </sst>
 </file>
@@ -222,12 +337,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -242,12 +375,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -584,21 +726,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B825CF8B-2BF9-274F-A235-D1B8BE2804AF}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="52.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="82.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="73.83203125" customWidth="1"/>
+    <col min="4" max="4" width="57.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" customWidth="1"/>
+    <col min="6" max="6" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -614,8 +757,11 @@
       <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -628,8 +774,11 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -642,8 +791,11 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="323" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -656,8 +808,11 @@
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -670,8 +825,11 @@
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -684,8 +842,11 @@
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -698,8 +859,11 @@
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -712,8 +876,11 @@
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -726,8 +893,11 @@
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F9" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="323" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -740,8 +910,11 @@
       <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -754,8 +927,11 @@
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F11" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -768,8 +944,11 @@
       <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F12" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -782,8 +961,11 @@
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -796,8 +978,11 @@
       <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="404" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -810,8 +995,11 @@
       <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F15" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -827,8 +1015,11 @@
       <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="F16" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -844,8 +1035,11 @@
       <c r="E17" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="F17" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -861,8 +1055,11 @@
       <c r="E18" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F18" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -877,6 +1074,9 @@
       </c>
       <c r="E19" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>